<commit_message>
UDF test - not yet working
</commit_message>
<xml_diff>
--- a/ExcelTests.xlsx
+++ b/ExcelTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oliver\Documents\VSCode\Node\MyExcelUDF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9032AE5-3F1B-4F5D-9B72-EFBB2667AA83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA57AC1-81DA-4A8A-B680-0004FBBDC2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -348,7 +348,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="1" width="752" row="8">
+  <wetp:taskpane dockstate="right" visibility="1" width="525" row="8">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
   <wetp:taskpane dockstate="right" visibility="0" width="0" row="0">
@@ -367,6 +367,19 @@
   <we:properties/>
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_UDF_ADD</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_UDF_CLOCK</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_UDF_INCREMENT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_UDF_LOG</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
 </we:webextension>
 </file>
 
@@ -408,7 +421,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>